<commit_message>
PS study progress: 10 2651
</commit_message>
<xml_diff>
--- a/computer_skills/各种快捷键总结.xlsx
+++ b/computer_skills/各种快捷键总结.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="1980" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="windows" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="247">
   <si>
     <t>组合</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -691,10 +691,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（个人喜好）快捷键整理，作者：李英俊小朋友，仅供参考，基于PS 2014 CC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Q</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -802,10 +798,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>（个人喜好）快捷键整理，作者：李英俊小朋友，仅供参考，基于PR 2014 CC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>时间轴 前进和后退</t>
   </si>
   <si>
@@ -890,6 +882,126 @@
   </si>
   <si>
     <t>参考链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左键单击</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击图层小眼睛，隐藏其他图层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>再次点击，恢复刚才隐藏的图层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图层向下移动一层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图层向上移动一层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图层移动到当前组的最下面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图层移动到当前组的最上面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左键拖动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复制图层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以复制多个图层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同上</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩小</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按屏幕大小缩放</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等同于双击抓手工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按实际像素缩放（100%）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>等同于双击缩放工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>空格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抓手工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>缩小工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放大工具</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（个人喜好）快捷键整理，作者：李英俊小朋友，仅供参考，基于PS 2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（个人喜好）快捷键整理，作者：李英俊小朋友，仅供参考，基于PR 2021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图层编组</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -897,7 +1009,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -927,6 +1039,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -949,7 +1070,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1008,6 +1129,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1015,6 +1148,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1309,27 +1510,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="13" t="s">
         <v>1</v>
       </c>
@@ -1517,10 +1718,10 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="F21" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>194</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1554,27 +1755,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1987,7 +2188,7 @@
       <c r="F41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="G41" s="20" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2001,7 +2202,7 @@
       <c r="F42" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G42" s="18"/>
+      <c r="G42" s="20"/>
     </row>
     <row r="43" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
@@ -2010,7 +2211,7 @@
       <c r="F43" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G43" s="18"/>
+      <c r="G43" s="20"/>
     </row>
     <row r="44" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
@@ -2190,16 +2391,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="4" t="s">
         <v>157</v>
       </c>
@@ -2211,12 +2412,12 @@
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2516,16 +2717,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
       <c r="I1" s="11" t="s">
         <v>157</v>
       </c>
@@ -2537,12 +2738,12 @@
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="11" t="s">
         <v>1</v>
       </c>
@@ -2618,7 +2819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -2632,27 +2833,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2677,7 +2878,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
@@ -2735,40 +2936,44 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="18"/>
+    <col min="7" max="7" width="34" style="18" customWidth="1"/>
+    <col min="8" max="8" width="53.5" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="A1" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
@@ -2792,6 +2997,7 @@
       <c r="E3" s="17" t="s">
         <v>15</v>
       </c>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
@@ -2802,10 +3008,10 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H4" s="14"/>
     </row>
@@ -2818,68 +3024,68 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="D6" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -2888,18 +3094,18 @@
         <v>3</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>173</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2907,17 +3113,17 @@
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>180</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2925,17 +3131,17 @@
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="H11" s="14" t="s">
         <v>183</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2945,10 +3151,10 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>186</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>187</v>
       </c>
       <c r="H12" s="14"/>
     </row>
@@ -2959,10 +3165,10 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>188</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>189</v>
       </c>
       <c r="H13" s="14"/>
     </row>
@@ -2975,10 +3181,10 @@
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H14" s="14"/>
     </row>
@@ -2992,10 +3198,10 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -3012,7 +3218,7 @@
         <v>84</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H16" s="14"/>
     </row>
@@ -3025,10 +3231,10 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H17" s="14"/>
     </row>
@@ -3041,10 +3247,10 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H18" s="14"/>
     </row>
@@ -3059,10 +3265,10 @@
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>205</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>207</v>
       </c>
       <c r="H19" s="14"/>
     </row>
@@ -3079,10 +3285,10 @@
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H20" s="14"/>
     </row>
@@ -3095,10 +3301,10 @@
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H21" s="14"/>
     </row>
@@ -3113,10 +3319,10 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H22" s="14"/>
     </row>
@@ -3127,10 +3333,10 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
       <c r="F23" s="12" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H23" s="14"/>
     </row>
@@ -3144,24 +3350,199 @@
         <v>83</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G24" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="H24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="H24" s="14"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H25" s="15"/>
+      <c r="G25" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H26" s="15"/>
+      <c r="B26" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H27" s="15"/>
+      <c r="B27" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H28" s="15"/>
+      <c r="B28" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C30" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="H31" s="22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="F34" s="18">
+        <v>0</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="18">
+        <v>0</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F36" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C37" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G38" s="18" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>246</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3176,10 +3557,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3189,27 +3573,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="A1" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="13" t="s">
         <v>1</v>
       </c>
@@ -3241,10 +3625,10 @@
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H4" s="14"/>
     </row>
@@ -3257,10 +3641,10 @@
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H5" s="14"/>
     </row>
@@ -3270,10 +3654,10 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H6" s="14"/>
     </row>
@@ -3284,10 +3668,10 @@
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H7" s="14"/>
     </row>

</xml_diff>

<commit_message>
study in P14 0411
</commit_message>
<xml_diff>
--- a/computer_skills/各种快捷键总结.xlsx
+++ b/computer_skills/各种快捷键总结.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
+    <workbookView xWindow="3030" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="windows" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="264">
   <si>
     <t>组合</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -925,10 +925,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>复制图层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>可以复制多个图层</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1002,6 +998,78 @@
   </si>
   <si>
     <t>图层编组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开/关闭辅助线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剪切图层到新的图层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>复制图层到新的图层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消选区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重新选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择反向</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示/隐藏辅助线、选区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前景色填充</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改羽化值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示/隐藏 标尺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>背景色填充</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1070,7 +1138,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1139,6 +1207,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1510,27 +1581,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="13" t="s">
         <v>1</v>
       </c>
@@ -1755,27 +1826,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2188,7 +2259,7 @@
       <c r="F41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G41" s="24" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2202,7 +2273,7 @@
       <c r="F42" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G42" s="20"/>
+      <c r="G42" s="24"/>
     </row>
     <row r="43" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
@@ -2211,7 +2282,7 @@
       <c r="F43" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G43" s="20"/>
+      <c r="G43" s="24"/>
     </row>
     <row r="44" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
@@ -2391,16 +2462,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="4" t="s">
         <v>157</v>
       </c>
@@ -2412,12 +2483,12 @@
       <c r="A2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
@@ -2717,16 +2788,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="11" t="s">
         <v>157</v>
       </c>
@@ -2738,12 +2809,12 @@
       <c r="A2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="11" t="s">
         <v>1</v>
       </c>
@@ -2833,27 +2904,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -2939,10 +3010,10 @@
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2953,27 +3024,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="A1" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="12" t="s">
         <v>1</v>
       </c>
@@ -3429,10 +3500,10 @@
         <v>226</v>
       </c>
       <c r="G30" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H30" s="14" t="s">
         <v>227</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3440,97 +3511,101 @@
         <v>3</v>
       </c>
       <c r="F31" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H31" s="22" t="s">
         <v>229</v>
       </c>
-      <c r="G31" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="H31" s="22" t="s">
-        <v>230</v>
-      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>233</v>
-      </c>
+      <c r="B32" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" s="22"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B33" s="18" t="s">
         <v>3</v>
       </c>
       <c r="F33" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>232</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B34" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="F34" s="18">
-        <v>0</v>
+      <c r="F34" s="23" t="s">
+        <v>231</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B35" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="C35" s="18"/>
       <c r="F35" s="18">
         <v>0</v>
       </c>
       <c r="G35" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="18">
+        <v>0</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="H36" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="H35" s="15" t="s">
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F37" s="18" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="F36" s="18" t="s">
+      <c r="G37" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="G36" s="18" t="s">
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C38" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="G38" s="18" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C37" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
@@ -3538,10 +3613,128 @@
         <v>3</v>
       </c>
       <c r="F39" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="G40" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="G39" s="18" t="s">
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="18" t="s">
         <v>246</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="G44" s="18" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F45" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="20"/>
+      <c r="C47" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="20"/>
+      <c r="F48" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D49" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -3573,27 +3766,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
-        <v>244</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="A1" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="F2" s="13" t="s">
         <v>1</v>
       </c>

</xml_diff>